<commit_message>
Added textBox Test and starter working on radio button and check box page and test
</commit_message>
<xml_diff>
--- a/src/test/java/DemoQaData.xlsx
+++ b/src/test/java/DemoQaData.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="URL" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="TextBox" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="TextBoxInvalidEmail" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">HomeUrl</t>
   </si>
@@ -57,6 +58,12 @@
   </si>
   <si>
     <t xml:space="preserve">Trenutna Adresa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InvalidEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@pera.com</t>
   </si>
 </sst>
 </file>
@@ -228,8 +235,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -280,4 +287,38 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Logo, Profile and SideBar Tests. Also, previous tests updated with additional cases
</commit_message>
<xml_diff>
--- a/src/test/java/DemoQaData.xlsx
+++ b/src/test/java/DemoQaData.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="URL" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="TextBox" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="TextBoxInvalidEmail" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="BookStoreLogIn" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">HomeUrl</t>
   </si>
@@ -64,6 +65,27 @@
   </si>
   <si>
     <t xml:space="preserve">@pera.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">peracom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/pera@pera.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pera.com@</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ValidUsername</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ValidPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">helenatodorovic86@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITBootcamp2023!</t>
   </si>
 </sst>
 </file>
@@ -151,7 +173,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -169,6 +191,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -294,25 +324,93 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.71"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" display="/pera@pera.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.22"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>13</v>
+      <c r="A2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="helenatodorovic86@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>